<commit_message>
CSV of raw data updated with dry 2020 runs
</commit_message>
<xml_diff>
--- a/BG_Paper/data/FCE_SI_data_xls_11_July_2023_Sturges_edits.xlsx
+++ b/BG_Paper/data/FCE_SI_data_xls_11_July_2023_Sturges_edits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17035\Desktop\New GitHub\BG_Paper\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17035\Desktop\New GitHub\Brown-vs-Green\BG_Paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E6C74C-B253-40CE-A5A8-52E5D80E8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3821553-1C6F-483F-B5B8-F0D6531D1BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="765" windowWidth="24450" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -38057,7 +38057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -38601,8 +38601,8 @@
   <dimension ref="A1:Y984"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A936" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C965" activeCellId="2" sqref="A967:XFD967 A968:XFD968 A965:XFD965"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -98696,7 +98696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B51579-D869-4099-BF83-BC624C34CAFB}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>

</xml_diff>